<commit_message>
0.0.22: Adapt array of enumemerate.
</commit_message>
<xml_diff>
--- a/meta/test4/PostEnumStatusSample.xlsx
+++ b/meta/test4/PostEnumStatusSample.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestAutotest/meta/test4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B142046-A9B4-DA41-AEBD-489B83054BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C1CC3E-8B84-4443-BF2F-4BCCD927ADB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="500" windowWidth="26200" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13760" yWindow="1600" windowWidth="26200" windowHeight="17500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase" sheetId="8" r:id="rId1"/>
     <sheet name="PostEnumStatusSamplePostTest" sheetId="15" r:id="rId2"/>
     <sheet name="GetEnumCodeSamplePostTest" sheetId="16" r:id="rId3"/>
-    <sheet name="Config" sheetId="7" r:id="rId4"/>
+    <sheet name="PostEnumStatusArraySampleTest" sheetId="18" r:id="rId4"/>
+    <sheet name="Config" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="119">
   <si>
     <t>2.定義書様式に記入された情報から、メタファイルをXMLファイルに変換する処理の定義に相当するJavaソースコードが自動生成されます。</t>
   </si>
@@ -626,6 +627,44 @@
   </si>
   <si>
     <t>CODE04</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>PostEnumStatusArraySample</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>配列の設定</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ハイレツ </t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t xml:space="preserve">セッテイ </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>PostEnumStatusArraySample</t>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <t>このクラスは、PostEnumStatusArraySampleのためのJUnit処理を定義します。</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>#</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>result[]</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>Ok</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>oK</t>
     <phoneticPr fontId="12"/>
   </si>
 </sst>
@@ -1842,7 +1881,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2212,13 +2251,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2668,8 +2701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B86D5CC-26D4-0349-B89F-A4BFBE2080C4}">
   <dimension ref="A1:W1044"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView topLeftCell="J2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="T31" sqref="T31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -2785,11 +2818,11 @@
         <v>31</v>
       </c>
       <c r="B9" s="90"/>
-      <c r="C9" s="157" t="s">
+      <c r="C9" s="155" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="158"/>
-      <c r="E9" s="158"/>
+      <c r="D9" s="156"/>
+      <c r="E9" s="156"/>
       <c r="F9" s="93"/>
       <c r="G9" s="94"/>
       <c r="H9" s="77"/>
@@ -2911,33 +2944,33 @@
       <c r="W18" s="5"/>
     </row>
     <row r="19" spans="1:23" ht="12.75" customHeight="1">
-      <c r="A19" s="137"/>
-      <c r="B19" s="138"/>
-      <c r="C19" s="138"/>
-      <c r="D19" s="138"/>
-      <c r="E19" s="138"/>
-      <c r="F19" s="138"/>
-      <c r="G19" s="138"/>
-      <c r="H19" s="138"/>
-      <c r="I19" s="138"/>
-      <c r="J19" s="138"/>
-      <c r="K19" s="138"/>
-      <c r="L19" s="139"/>
-      <c r="M19" s="177" t="s">
+      <c r="A19" s="135"/>
+      <c r="B19" s="136"/>
+      <c r="C19" s="136"/>
+      <c r="D19" s="136"/>
+      <c r="E19" s="136"/>
+      <c r="F19" s="136"/>
+      <c r="G19" s="136"/>
+      <c r="H19" s="136"/>
+      <c r="I19" s="136"/>
+      <c r="J19" s="136"/>
+      <c r="K19" s="136"/>
+      <c r="L19" s="137"/>
+      <c r="M19" s="175" t="s">
         <v>41</v>
       </c>
-      <c r="N19" s="178"/>
-      <c r="O19" s="178"/>
-      <c r="P19" s="178"/>
-      <c r="Q19" s="178"/>
-      <c r="R19" s="177" t="s">
+      <c r="N19" s="176"/>
+      <c r="O19" s="176"/>
+      <c r="P19" s="176"/>
+      <c r="Q19" s="176"/>
+      <c r="R19" s="175" t="s">
         <v>42</v>
       </c>
-      <c r="S19" s="178"/>
-      <c r="T19" s="178"/>
-      <c r="U19" s="178"/>
-      <c r="V19" s="178"/>
-      <c r="W19" s="140"/>
+      <c r="S19" s="176"/>
+      <c r="T19" s="176"/>
+      <c r="U19" s="176"/>
+      <c r="V19" s="176"/>
+      <c r="W19" s="138"/>
     </row>
     <row r="20" spans="1:23" ht="12.75" customHeight="1">
       <c r="A20" s="116"/>
@@ -2953,91 +2986,91 @@
       <c r="I20" s="116"/>
       <c r="J20" s="116"/>
       <c r="K20" s="116"/>
-      <c r="L20" s="141"/>
-      <c r="M20" s="175" t="s">
+      <c r="L20" s="139"/>
+      <c r="M20" s="173" t="s">
         <v>63</v>
       </c>
-      <c r="N20" s="176"/>
-      <c r="O20" s="176"/>
-      <c r="P20" s="176"/>
-      <c r="Q20" s="176"/>
-      <c r="R20" s="175" t="s">
+      <c r="N20" s="174"/>
+      <c r="O20" s="174"/>
+      <c r="P20" s="174"/>
+      <c r="Q20" s="174"/>
+      <c r="R20" s="173" t="s">
         <v>63</v>
       </c>
-      <c r="S20" s="176"/>
-      <c r="T20" s="176"/>
-      <c r="U20" s="176"/>
-      <c r="V20" s="176"/>
+      <c r="S20" s="174"/>
+      <c r="T20" s="174"/>
+      <c r="U20" s="174"/>
+      <c r="V20" s="174"/>
       <c r="W20" s="116"/>
     </row>
     <row r="21" spans="1:23" ht="23" customHeight="1">
-      <c r="A21" s="155" t="s">
+      <c r="A21" s="153" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="155" t="s">
+      <c r="B21" s="153" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="156" t="s">
+      <c r="C21" s="154" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="156" t="s">
+      <c r="D21" s="154" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="155" t="s">
+      <c r="E21" s="153" t="s">
         <v>29</v>
       </c>
-      <c r="F21" s="155" t="s">
+      <c r="F21" s="153" t="s">
         <v>51</v>
       </c>
-      <c r="G21" s="155" t="s">
+      <c r="G21" s="153" t="s">
         <v>47</v>
       </c>
-      <c r="H21" s="155" t="s">
+      <c r="H21" s="153" t="s">
         <v>32</v>
       </c>
-      <c r="I21" s="155" t="s">
+      <c r="I21" s="153" t="s">
         <v>46</v>
       </c>
-      <c r="J21" s="155" t="s">
+      <c r="J21" s="153" t="s">
         <v>49</v>
       </c>
-      <c r="K21" s="155" t="s">
+      <c r="K21" s="153" t="s">
         <v>52</v>
       </c>
-      <c r="L21" s="159" t="s">
+      <c r="L21" s="157" t="s">
         <v>45</v>
       </c>
-      <c r="M21" s="155" t="s">
+      <c r="M21" s="153" t="s">
         <v>64</v>
       </c>
-      <c r="N21" s="155" t="s">
+      <c r="N21" s="153" t="s">
         <v>65</v>
       </c>
-      <c r="O21" s="155" t="s">
+      <c r="O21" s="153" t="s">
         <v>66</v>
       </c>
-      <c r="P21" s="155" t="s">
+      <c r="P21" s="153" t="s">
         <v>67</v>
       </c>
-      <c r="Q21" s="155" t="s">
+      <c r="Q21" s="153" t="s">
         <v>68</v>
       </c>
-      <c r="R21" s="155" t="s">
+      <c r="R21" s="153" t="s">
         <v>69</v>
       </c>
-      <c r="S21" s="155" t="s">
+      <c r="S21" s="153" t="s">
         <v>70</v>
       </c>
-      <c r="T21" s="155" t="s">
+      <c r="T21" s="153" t="s">
         <v>71</v>
       </c>
-      <c r="U21" s="155" t="s">
+      <c r="U21" s="153" t="s">
         <v>72</v>
       </c>
-      <c r="V21" s="155" t="s">
+      <c r="V21" s="153" t="s">
         <v>73</v>
       </c>
-      <c r="W21" s="155" t="s">
+      <c r="W21" s="153" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3049,7 +3082,7 @@
         <v>95</v>
       </c>
       <c r="C22" s="18"/>
-      <c r="D22" s="146" t="s">
+      <c r="D22" s="144" t="s">
         <v>85</v>
       </c>
       <c r="E22" s="18" t="s">
@@ -3063,29 +3096,29 @@
       <c r="I22" s="119"/>
       <c r="J22" s="119"/>
       <c r="K22" s="119"/>
-      <c r="L22" s="148">
+      <c r="L22" s="146">
         <v>1</v>
       </c>
-      <c r="M22" s="149"/>
-      <c r="N22" s="150"/>
-      <c r="O22" s="151" t="s">
+      <c r="M22" s="147"/>
+      <c r="N22" s="148"/>
+      <c r="O22" s="149" t="s">
         <v>36</v>
       </c>
-      <c r="P22" s="151" t="s">
+      <c r="P22" s="149" t="s">
         <v>37</v>
       </c>
-      <c r="Q22" s="149" t="s">
+      <c r="Q22" s="147" t="s">
         <v>38</v>
       </c>
-      <c r="R22" s="149"/>
-      <c r="S22" s="150"/>
-      <c r="T22" s="151" t="s">
+      <c r="R22" s="147"/>
+      <c r="S22" s="148"/>
+      <c r="T22" s="149" t="s">
         <v>36</v>
       </c>
-      <c r="U22" s="151" t="s">
+      <c r="U22" s="149" t="s">
         <v>37</v>
       </c>
-      <c r="V22" s="149" t="s">
+      <c r="V22" s="147" t="s">
         <v>38</v>
       </c>
       <c r="W22" s="37"/>
@@ -3099,7 +3132,7 @@
         <v>96</v>
       </c>
       <c r="C23" s="18"/>
-      <c r="D23" s="146" t="s">
+      <c r="D23" s="144" t="s">
         <v>85</v>
       </c>
       <c r="E23" s="18" t="s">
@@ -3113,43 +3146,43 @@
       <c r="I23" s="119"/>
       <c r="J23" s="119"/>
       <c r="K23" s="119"/>
-      <c r="L23" s="148">
+      <c r="L23" s="146">
         <v>2</v>
       </c>
-      <c r="M23" s="149"/>
-      <c r="N23" s="150"/>
-      <c r="O23" s="151" t="s">
+      <c r="M23" s="147"/>
+      <c r="N23" s="148"/>
+      <c r="O23" s="149" t="s">
         <v>36</v>
       </c>
-      <c r="P23" s="151" t="s">
+      <c r="P23" s="149" t="s">
         <v>37</v>
       </c>
-      <c r="Q23" s="149" t="s">
+      <c r="Q23" s="147" t="s">
         <v>38</v>
       </c>
-      <c r="R23" s="149"/>
-      <c r="S23" s="150"/>
-      <c r="T23" s="151" t="s">
+      <c r="R23" s="147"/>
+      <c r="S23" s="148"/>
+      <c r="T23" s="149" t="s">
         <v>36</v>
       </c>
-      <c r="U23" s="151" t="s">
+      <c r="U23" s="149" t="s">
         <v>37</v>
       </c>
-      <c r="V23" s="149" t="s">
+      <c r="V23" s="147" t="s">
         <v>38</v>
       </c>
       <c r="W23" s="37"/>
     </row>
     <row r="24" spans="1:23" ht="12.75" customHeight="1">
       <c r="A24" s="37">
-        <f t="shared" ref="A24:A31" si="0">A23+1</f>
+        <f t="shared" ref="A24:A30" si="0">A23+1</f>
         <v>3</v>
       </c>
       <c r="B24" s="97" t="s">
         <v>97</v>
       </c>
       <c r="C24" s="18"/>
-      <c r="D24" s="146" t="s">
+      <c r="D24" s="144" t="s">
         <v>85</v>
       </c>
       <c r="E24" s="18" t="s">
@@ -3163,29 +3196,29 @@
       <c r="I24" s="119"/>
       <c r="J24" s="119"/>
       <c r="K24" s="119"/>
-      <c r="L24" s="148">
+      <c r="L24" s="146">
         <v>3</v>
       </c>
-      <c r="M24" s="149"/>
-      <c r="N24" s="150"/>
-      <c r="O24" s="151" t="s">
+      <c r="M24" s="147"/>
+      <c r="N24" s="148"/>
+      <c r="O24" s="149" t="s">
         <v>36</v>
       </c>
-      <c r="P24" s="151" t="s">
+      <c r="P24" s="149" t="s">
         <v>37</v>
       </c>
-      <c r="Q24" s="149" t="s">
+      <c r="Q24" s="147" t="s">
         <v>38</v>
       </c>
-      <c r="R24" s="149"/>
-      <c r="S24" s="150"/>
-      <c r="T24" s="151" t="s">
+      <c r="R24" s="147"/>
+      <c r="S24" s="148"/>
+      <c r="T24" s="149" t="s">
         <v>36</v>
       </c>
-      <c r="U24" s="151" t="s">
+      <c r="U24" s="149" t="s">
         <v>37</v>
       </c>
-      <c r="V24" s="149" t="s">
+      <c r="V24" s="147" t="s">
         <v>38</v>
       </c>
       <c r="W24" s="37"/>
@@ -3199,7 +3232,7 @@
         <v>98</v>
       </c>
       <c r="C25" s="18"/>
-      <c r="D25" s="146" t="s">
+      <c r="D25" s="144" t="s">
         <v>85</v>
       </c>
       <c r="E25" s="18" t="s">
@@ -3213,29 +3246,29 @@
       <c r="I25" s="119"/>
       <c r="J25" s="119"/>
       <c r="K25" s="119"/>
-      <c r="L25" s="148">
+      <c r="L25" s="146">
         <v>4</v>
       </c>
-      <c r="M25" s="149"/>
-      <c r="N25" s="150"/>
-      <c r="O25" s="151" t="s">
+      <c r="M25" s="147"/>
+      <c r="N25" s="148"/>
+      <c r="O25" s="149" t="s">
         <v>36</v>
       </c>
-      <c r="P25" s="151" t="s">
+      <c r="P25" s="149" t="s">
         <v>37</v>
       </c>
-      <c r="Q25" s="149" t="s">
+      <c r="Q25" s="147" t="s">
         <v>38</v>
       </c>
-      <c r="R25" s="149"/>
-      <c r="S25" s="150"/>
-      <c r="T25" s="151" t="s">
+      <c r="R25" s="147"/>
+      <c r="S25" s="148"/>
+      <c r="T25" s="149" t="s">
         <v>36</v>
       </c>
-      <c r="U25" s="151" t="s">
+      <c r="U25" s="149" t="s">
         <v>37</v>
       </c>
-      <c r="V25" s="149" t="s">
+      <c r="V25" s="147" t="s">
         <v>38</v>
       </c>
       <c r="W25" s="37"/>
@@ -3249,7 +3282,7 @@
         <v>99</v>
       </c>
       <c r="C26" s="18"/>
-      <c r="D26" s="143" t="s">
+      <c r="D26" s="141" t="s">
         <v>103</v>
       </c>
       <c r="E26" s="18" t="s">
@@ -3263,29 +3296,29 @@
       <c r="I26" s="119"/>
       <c r="J26" s="119"/>
       <c r="K26" s="119"/>
-      <c r="L26" s="148">
+      <c r="L26" s="146">
         <v>1</v>
       </c>
-      <c r="M26" s="149"/>
-      <c r="N26" s="150"/>
-      <c r="O26" s="151" t="s">
+      <c r="M26" s="147"/>
+      <c r="N26" s="148"/>
+      <c r="O26" s="149" t="s">
         <v>36</v>
       </c>
-      <c r="P26" s="151" t="s">
+      <c r="P26" s="149" t="s">
         <v>37</v>
       </c>
-      <c r="Q26" s="149" t="s">
+      <c r="Q26" s="147" t="s">
         <v>38</v>
       </c>
-      <c r="R26" s="149"/>
-      <c r="S26" s="150"/>
-      <c r="T26" s="151" t="s">
+      <c r="R26" s="147"/>
+      <c r="S26" s="148"/>
+      <c r="T26" s="149" t="s">
         <v>36</v>
       </c>
-      <c r="U26" s="151" t="s">
+      <c r="U26" s="149" t="s">
         <v>37</v>
       </c>
-      <c r="V26" s="149" t="s">
+      <c r="V26" s="147" t="s">
         <v>38</v>
       </c>
       <c r="W26" s="37"/>
@@ -3299,7 +3332,7 @@
         <v>100</v>
       </c>
       <c r="C27" s="16"/>
-      <c r="D27" s="143" t="s">
+      <c r="D27" s="141" t="s">
         <v>103</v>
       </c>
       <c r="E27" s="18" t="s">
@@ -3313,29 +3346,29 @@
       <c r="I27" s="22"/>
       <c r="J27" s="22"/>
       <c r="K27" s="22"/>
-      <c r="L27" s="148">
+      <c r="L27" s="146">
         <v>2</v>
       </c>
       <c r="M27" s="127"/>
       <c r="N27" s="129"/>
-      <c r="O27" s="151" t="s">
+      <c r="O27" s="149" t="s">
         <v>36</v>
       </c>
-      <c r="P27" s="151" t="s">
+      <c r="P27" s="149" t="s">
         <v>37</v>
       </c>
-      <c r="Q27" s="149" t="s">
+      <c r="Q27" s="147" t="s">
         <v>38</v>
       </c>
       <c r="R27" s="127"/>
       <c r="S27" s="129"/>
-      <c r="T27" s="151" t="s">
+      <c r="T27" s="149" t="s">
         <v>36</v>
       </c>
-      <c r="U27" s="151" t="s">
+      <c r="U27" s="149" t="s">
         <v>37</v>
       </c>
-      <c r="V27" s="149" t="s">
+      <c r="V27" s="147" t="s">
         <v>38</v>
       </c>
       <c r="W27" s="37"/>
@@ -3349,7 +3382,7 @@
         <v>101</v>
       </c>
       <c r="C28" s="18"/>
-      <c r="D28" s="143" t="s">
+      <c r="D28" s="141" t="s">
         <v>103</v>
       </c>
       <c r="E28" s="18" t="s">
@@ -3363,29 +3396,29 @@
       <c r="I28" s="22"/>
       <c r="J28" s="22"/>
       <c r="K28" s="22"/>
-      <c r="L28" s="148">
+      <c r="L28" s="146">
         <v>3</v>
       </c>
       <c r="M28" s="126"/>
       <c r="N28" s="130"/>
-      <c r="O28" s="151" t="s">
+      <c r="O28" s="149" t="s">
         <v>36</v>
       </c>
-      <c r="P28" s="151" t="s">
+      <c r="P28" s="149" t="s">
         <v>37</v>
       </c>
-      <c r="Q28" s="149" t="s">
+      <c r="Q28" s="147" t="s">
         <v>38</v>
       </c>
       <c r="R28" s="126"/>
       <c r="S28" s="130"/>
-      <c r="T28" s="151" t="s">
+      <c r="T28" s="149" t="s">
         <v>36</v>
       </c>
-      <c r="U28" s="151" t="s">
+      <c r="U28" s="149" t="s">
         <v>37</v>
       </c>
-      <c r="V28" s="149" t="s">
+      <c r="V28" s="147" t="s">
         <v>38</v>
       </c>
       <c r="W28" s="18"/>
@@ -3399,7 +3432,7 @@
         <v>102</v>
       </c>
       <c r="C29" s="18"/>
-      <c r="D29" s="143" t="s">
+      <c r="D29" s="141" t="s">
         <v>103</v>
       </c>
       <c r="E29" s="18" t="s">
@@ -3413,63 +3446,88 @@
       <c r="I29" s="22"/>
       <c r="J29" s="22"/>
       <c r="K29" s="22"/>
-      <c r="L29" s="148">
+      <c r="L29" s="146">
         <v>4</v>
       </c>
       <c r="M29" s="126"/>
       <c r="N29" s="130"/>
-      <c r="O29" s="151" t="s">
+      <c r="O29" s="149" t="s">
         <v>36</v>
       </c>
-      <c r="P29" s="151" t="s">
+      <c r="P29" s="149" t="s">
         <v>37</v>
       </c>
-      <c r="Q29" s="149" t="s">
+      <c r="Q29" s="147" t="s">
         <v>38</v>
       </c>
       <c r="R29" s="126"/>
       <c r="S29" s="130"/>
-      <c r="T29" s="151" t="s">
+      <c r="T29" s="149" t="s">
         <v>36</v>
       </c>
-      <c r="U29" s="151" t="s">
+      <c r="U29" s="149" t="s">
         <v>37</v>
       </c>
-      <c r="V29" s="149" t="s">
+      <c r="V29" s="147" t="s">
         <v>38</v>
       </c>
       <c r="W29" s="97"/>
     </row>
     <row r="30" spans="1:23" ht="12.75" customHeight="1">
-      <c r="A30" s="37"/>
-      <c r="B30" s="144"/>
+      <c r="A30" s="37">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B30" s="142" t="s">
+        <v>112</v>
+      </c>
       <c r="C30" s="18"/>
-      <c r="D30" s="144"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
+      <c r="D30" s="142" t="s">
+        <v>113</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30" s="18" t="b">
+        <v>0</v>
+      </c>
       <c r="G30" s="18"/>
       <c r="H30" s="22"/>
       <c r="I30" s="22"/>
       <c r="J30" s="22"/>
       <c r="K30" s="22"/>
-      <c r="L30" s="18"/>
+      <c r="L30" s="18">
+        <v>1</v>
+      </c>
       <c r="M30" s="126"/>
       <c r="N30" s="131"/>
-      <c r="O30" s="133"/>
-      <c r="P30" s="135"/>
-      <c r="Q30" s="126"/>
+      <c r="O30" s="149" t="s">
+        <v>36</v>
+      </c>
+      <c r="P30" s="149" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q30" s="147" t="s">
+        <v>38</v>
+      </c>
       <c r="R30" s="126"/>
       <c r="S30" s="131"/>
-      <c r="T30" s="133"/>
-      <c r="U30" s="135"/>
-      <c r="V30" s="126"/>
-      <c r="W30" s="154"/>
+      <c r="T30" s="149" t="s">
+        <v>36</v>
+      </c>
+      <c r="U30" s="149" t="s">
+        <v>37</v>
+      </c>
+      <c r="V30" s="147" t="s">
+        <v>38</v>
+      </c>
+      <c r="W30" s="152"/>
     </row>
     <row r="31" spans="1:23" ht="12.75" customHeight="1">
       <c r="A31" s="37"/>
-      <c r="B31" s="142"/>
+      <c r="B31" s="140"/>
       <c r="C31" s="13"/>
-      <c r="D31" s="147"/>
+      <c r="D31" s="145"/>
       <c r="E31" s="18"/>
       <c r="F31" s="122"/>
       <c r="G31" s="13"/>
@@ -3480,21 +3538,21 @@
       <c r="L31" s="13"/>
       <c r="M31" s="126"/>
       <c r="N31" s="131"/>
-      <c r="O31" s="134"/>
-      <c r="P31" s="136"/>
+      <c r="O31" s="133"/>
+      <c r="P31" s="134"/>
       <c r="Q31" s="126"/>
       <c r="R31" s="126"/>
       <c r="S31" s="131"/>
-      <c r="T31" s="134"/>
-      <c r="U31" s="136"/>
+      <c r="T31" s="133"/>
+      <c r="U31" s="134"/>
       <c r="V31" s="126"/>
-      <c r="W31" s="153"/>
+      <c r="W31" s="151"/>
     </row>
     <row r="32" spans="1:23" ht="12.75" customHeight="1">
       <c r="A32" s="16"/>
       <c r="B32" s="96"/>
       <c r="C32" s="16"/>
-      <c r="D32" s="145"/>
+      <c r="D32" s="143"/>
       <c r="E32" s="16"/>
       <c r="F32" s="16"/>
       <c r="G32" s="16"/>
@@ -5676,7 +5734,7 @@
         <v>80</v>
       </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="152"/>
+      <c r="C11" s="150"/>
       <c r="D11" s="12">
         <v>1</v>
       </c>
@@ -5687,11 +5745,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="164" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A12" s="171" t="s">
+    <row r="12" spans="1:7" s="162" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A12" s="169" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="172" t="s">
+      <c r="B12" s="170" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="82" t="s">
@@ -5705,172 +5763,172 @@
         <f>"Input"&amp;E11</f>
         <v>Input2</v>
       </c>
-      <c r="F12" s="173" t="str">
+      <c r="F12" s="171" t="str">
         <f>"Expect"&amp;F11</f>
         <v>Expect1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="164" customFormat="1" ht="15" thickBot="1">
-      <c r="A13" s="161">
+    <row r="13" spans="1:7" s="162" customFormat="1" ht="15" thickBot="1">
+      <c r="A13" s="159">
         <v>1</v>
       </c>
-      <c r="B13" s="162" t="s">
+      <c r="B13" s="160" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="163"/>
-      <c r="D13" s="160" t="s">
+      <c r="C13" s="161"/>
+      <c r="D13" s="158" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="160" t="s">
+      <c r="E13" s="158" t="s">
         <v>88</v>
       </c>
-      <c r="F13" s="174" t="s">
+      <c r="F13" s="172" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="164" customFormat="1">
-      <c r="A14" s="161">
+    <row r="14" spans="1:7" s="162" customFormat="1">
+      <c r="A14" s="159">
         <f>A13+1</f>
         <v>2</v>
       </c>
-      <c r="B14" s="166" t="s">
+      <c r="B14" s="164" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="167"/>
-      <c r="D14" s="167"/>
-      <c r="E14" s="167"/>
-      <c r="F14" s="168" t="s">
+      <c r="C14" s="165"/>
+      <c r="D14" s="165"/>
+      <c r="E14" s="165"/>
+      <c r="F14" s="166" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="164" customFormat="1" ht="15" thickBot="1">
-      <c r="A15" s="161">
+    <row r="15" spans="1:7" s="162" customFormat="1" ht="15" thickBot="1">
+      <c r="A15" s="159">
         <f t="shared" ref="A15" si="0">A14+1</f>
         <v>3</v>
       </c>
-      <c r="B15" s="160" t="s">
+      <c r="B15" s="158" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="163">
+      <c r="C15" s="161">
         <v>1</v>
       </c>
-      <c r="D15" s="169">
+      <c r="D15" s="167">
         <v>1</v>
       </c>
-      <c r="E15" s="169" t="s">
+      <c r="E15" s="167" t="s">
         <v>91</v>
       </c>
-      <c r="F15" s="170" t="s">
+      <c r="F15" s="168" t="s">
         <v>90</v>
       </c>
       <c r="G15" s="78"/>
     </row>
-    <row r="16" spans="1:7" s="164" customFormat="1">
-      <c r="A16" s="161">
+    <row r="16" spans="1:7" s="162" customFormat="1">
+      <c r="A16" s="159">
         <f>A15+1</f>
         <v>4</v>
       </c>
-      <c r="B16" s="166" t="s">
+      <c r="B16" s="164" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="167"/>
-      <c r="D16" s="167"/>
-      <c r="E16" s="167"/>
-      <c r="F16" s="168" t="s">
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="166" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="164" customFormat="1" ht="15" thickBot="1">
-      <c r="A17" s="161">
+    <row r="17" spans="1:7" s="162" customFormat="1" ht="15" thickBot="1">
+      <c r="A17" s="159">
         <f t="shared" ref="A17:A19" si="1">A16+1</f>
         <v>5</v>
       </c>
       <c r="B17" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="165">
+      <c r="C17" s="163">
         <v>2</v>
       </c>
       <c r="D17" s="81">
         <v>2</v>
       </c>
-      <c r="E17" s="169" t="s">
+      <c r="E17" s="167" t="s">
         <v>92</v>
       </c>
-      <c r="F17" s="170" t="s">
+      <c r="F17" s="168" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="164" customFormat="1">
-      <c r="A18" s="161">
+    <row r="18" spans="1:7" s="162" customFormat="1">
+      <c r="A18" s="159">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B18" s="166" t="s">
+      <c r="B18" s="164" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="167"/>
-      <c r="D18" s="167"/>
-      <c r="E18" s="167"/>
-      <c r="F18" s="168" t="s">
+      <c r="C18" s="165"/>
+      <c r="D18" s="165"/>
+      <c r="E18" s="165"/>
+      <c r="F18" s="166" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="164" customFormat="1" ht="15" thickBot="1">
-      <c r="A19" s="161">
+    <row r="19" spans="1:7" s="162" customFormat="1" ht="15" thickBot="1">
+      <c r="A19" s="159">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B19" s="160" t="s">
+      <c r="B19" s="158" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="163">
+      <c r="C19" s="161">
         <v>3</v>
       </c>
-      <c r="D19" s="169">
+      <c r="D19" s="167">
         <v>3</v>
       </c>
-      <c r="E19" s="169" t="s">
+      <c r="E19" s="167" t="s">
         <v>93</v>
       </c>
-      <c r="F19" s="170" t="s">
+      <c r="F19" s="168" t="s">
         <v>90</v>
       </c>
       <c r="G19" s="78"/>
     </row>
-    <row r="20" spans="1:7" s="164" customFormat="1">
-      <c r="A20" s="161">
+    <row r="20" spans="1:7" s="162" customFormat="1">
+      <c r="A20" s="159">
         <f t="shared" ref="A20:A21" si="2">A19+1</f>
         <v>8</v>
       </c>
-      <c r="B20" s="166" t="s">
+      <c r="B20" s="164" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="167"/>
-      <c r="D20" s="167"/>
-      <c r="E20" s="167"/>
-      <c r="F20" s="168" t="s">
+      <c r="C20" s="165"/>
+      <c r="D20" s="165"/>
+      <c r="E20" s="165"/>
+      <c r="F20" s="166" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="164" customFormat="1">
-      <c r="A21" s="161">
+    <row r="21" spans="1:7" s="162" customFormat="1">
+      <c r="A21" s="159">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="B21" s="160" t="s">
+      <c r="B21" s="158" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="163">
+      <c r="C21" s="161">
         <v>4</v>
       </c>
-      <c r="D21" s="169">
+      <c r="D21" s="167">
         <v>4</v>
       </c>
-      <c r="E21" s="169" t="s">
+      <c r="E21" s="167" t="s">
         <v>94</v>
       </c>
-      <c r="F21" s="170" t="s">
+      <c r="F21" s="168" t="s">
         <v>90</v>
       </c>
       <c r="G21" s="78"/>
@@ -5897,7 +5955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFF2A7AE-16C8-214E-9094-18CF560FE160}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -5984,7 +6042,7 @@
         <v>80</v>
       </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="152"/>
+      <c r="C11" s="150"/>
       <c r="D11" s="12">
         <v>1</v>
       </c>
@@ -5992,11 +6050,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="164" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A12" s="171" t="s">
+    <row r="12" spans="1:5" s="162" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A12" s="169" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="172" t="s">
+      <c r="B12" s="170" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="82" t="s">
@@ -6006,151 +6064,151 @@
         <f>"Input"&amp;D11</f>
         <v>Input1</v>
       </c>
-      <c r="E12" s="173" t="str">
+      <c r="E12" s="171" t="str">
         <f>"Expect"&amp;E11</f>
         <v>Expect1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="164" customFormat="1" ht="15" thickBot="1">
-      <c r="A13" s="161">
+    <row r="13" spans="1:5" s="162" customFormat="1" ht="15" thickBot="1">
+      <c r="A13" s="159">
         <v>1</v>
       </c>
-      <c r="B13" s="162" t="s">
+      <c r="B13" s="160" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="163"/>
-      <c r="D13" s="160" t="s">
+      <c r="C13" s="161"/>
+      <c r="D13" s="158" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="174" t="s">
+      <c r="E13" s="172" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="164" customFormat="1">
-      <c r="A14" s="161">
+    <row r="14" spans="1:5" s="162" customFormat="1">
+      <c r="A14" s="159">
         <f>A13+1</f>
         <v>2</v>
       </c>
-      <c r="B14" s="166" t="s">
+      <c r="B14" s="164" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="167"/>
-      <c r="D14" s="167"/>
-      <c r="E14" s="168" t="s">
+      <c r="C14" s="165"/>
+      <c r="D14" s="165"/>
+      <c r="E14" s="166" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="164" customFormat="1" ht="15" thickBot="1">
-      <c r="A15" s="161">
+    <row r="15" spans="1:5" s="162" customFormat="1" ht="15" thickBot="1">
+      <c r="A15" s="159">
         <f t="shared" ref="A15" si="0">A14+1</f>
         <v>3</v>
       </c>
-      <c r="B15" s="160" t="s">
+      <c r="B15" s="158" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="163">
+      <c r="C15" s="161">
         <v>1</v>
       </c>
-      <c r="D15" s="169">
+      <c r="D15" s="167">
         <v>1</v>
       </c>
-      <c r="E15" s="170" t="s">
+      <c r="E15" s="168" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="164" customFormat="1">
-      <c r="A16" s="161">
+    <row r="16" spans="1:5" s="162" customFormat="1">
+      <c r="A16" s="159">
         <f>A15+1</f>
         <v>4</v>
       </c>
-      <c r="B16" s="166" t="s">
+      <c r="B16" s="164" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="167"/>
-      <c r="D16" s="167"/>
-      <c r="E16" s="168" t="s">
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="166" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="164" customFormat="1" ht="15" thickBot="1">
-      <c r="A17" s="161">
+    <row r="17" spans="1:5" s="162" customFormat="1" ht="15" thickBot="1">
+      <c r="A17" s="159">
         <f t="shared" ref="A17:A21" si="1">A16+1</f>
         <v>5</v>
       </c>
       <c r="B17" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="165">
+      <c r="C17" s="163">
         <v>2</v>
       </c>
       <c r="D17" s="81">
         <v>2</v>
       </c>
-      <c r="E17" s="170" t="s">
+      <c r="E17" s="168" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="164" customFormat="1">
-      <c r="A18" s="161">
+    <row r="18" spans="1:5" s="162" customFormat="1">
+      <c r="A18" s="159">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B18" s="166" t="s">
+      <c r="B18" s="164" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="167"/>
-      <c r="D18" s="167"/>
-      <c r="E18" s="168" t="s">
+      <c r="C18" s="165"/>
+      <c r="D18" s="165"/>
+      <c r="E18" s="166" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="164" customFormat="1" ht="15" thickBot="1">
-      <c r="A19" s="161">
+    <row r="19" spans="1:5" s="162" customFormat="1" ht="15" thickBot="1">
+      <c r="A19" s="159">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B19" s="160" t="s">
+      <c r="B19" s="158" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="163">
+      <c r="C19" s="161">
         <v>3</v>
       </c>
-      <c r="D19" s="169">
+      <c r="D19" s="167">
         <v>3</v>
       </c>
-      <c r="E19" s="170" t="s">
+      <c r="E19" s="168" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="164" customFormat="1">
-      <c r="A20" s="161">
+    <row r="20" spans="1:5" s="162" customFormat="1">
+      <c r="A20" s="159">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B20" s="166" t="s">
+      <c r="B20" s="164" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="167"/>
-      <c r="D20" s="167"/>
-      <c r="E20" s="168" t="s">
+      <c r="C20" s="165"/>
+      <c r="D20" s="165"/>
+      <c r="E20" s="166" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="164" customFormat="1">
-      <c r="A21" s="161">
+    <row r="21" spans="1:5" s="162" customFormat="1">
+      <c r="A21" s="159">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B21" s="160" t="s">
+      <c r="B21" s="158" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="163">
+      <c r="C21" s="161">
         <v>4</v>
       </c>
-      <c r="D21" s="169">
+      <c r="D21" s="167">
         <v>4</v>
       </c>
-      <c r="E21" s="170" t="s">
+      <c r="E21" s="168" t="s">
         <v>110</v>
       </c>
     </row>
@@ -6173,6 +6231,463 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C0D5C7-C156-324D-8CF0-5390E92B8446}">
+  <dimension ref="A1:G29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="5.1640625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="13" style="12" customWidth="1"/>
+    <col min="4" max="6" width="10.83203125" style="12"/>
+    <col min="7" max="7" width="10.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="78" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="78"/>
+    </row>
+    <row r="3" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="88"/>
+      <c r="C7" s="118" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="77"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="77"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="78"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="78"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="78"/>
+    </row>
+    <row r="11" spans="1:7" ht="15" thickBot="1">
+      <c r="A11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="150"/>
+      <c r="D11" s="12">
+        <v>1</v>
+      </c>
+      <c r="E11" s="12">
+        <v>2</v>
+      </c>
+      <c r="F11" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="162" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A12" s="169" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="170" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="82" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="79" t="str">
+        <f>"Input"&amp;D11</f>
+        <v>Input1</v>
+      </c>
+      <c r="E12" s="79" t="str">
+        <f>"Input"&amp;E11</f>
+        <v>Input2</v>
+      </c>
+      <c r="F12" s="171" t="str">
+        <f>"Expect"&amp;F11</f>
+        <v>Expect1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="162" customFormat="1" ht="15" thickBot="1">
+      <c r="A13" s="159">
+        <v>1</v>
+      </c>
+      <c r="B13" s="160" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="161"/>
+      <c r="D13" s="158" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="158" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" s="172" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="162" customFormat="1">
+      <c r="A14" s="159">
+        <f>A13+1</f>
+        <v>2</v>
+      </c>
+      <c r="B14" s="164" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="165"/>
+      <c r="D14" s="165"/>
+      <c r="E14" s="165"/>
+      <c r="F14" s="166" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="162" customFormat="1">
+      <c r="A15" s="159">
+        <f t="shared" ref="A15:A29" si="0">A14+1</f>
+        <v>3</v>
+      </c>
+      <c r="B15" s="158" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="161">
+        <v>1</v>
+      </c>
+      <c r="D15" s="167">
+        <v>1</v>
+      </c>
+      <c r="E15" s="167" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="168" t="s">
+        <v>90</v>
+      </c>
+      <c r="G15" s="78"/>
+    </row>
+    <row r="16" spans="1:7" s="162" customFormat="1">
+      <c r="A16" s="159">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B16" s="158" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="161"/>
+      <c r="D16" s="167"/>
+      <c r="E16" s="167" t="s">
+        <v>92</v>
+      </c>
+      <c r="F16" s="168" t="s">
+        <v>117</v>
+      </c>
+      <c r="G16" s="78"/>
+    </row>
+    <row r="17" spans="1:7" s="162" customFormat="1" ht="15" thickBot="1">
+      <c r="A17" s="159">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B17" s="158" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="161"/>
+      <c r="D17" s="167"/>
+      <c r="E17" s="167" t="s">
+        <v>115</v>
+      </c>
+      <c r="F17" s="168" t="s">
+        <v>115</v>
+      </c>
+      <c r="G17" s="78"/>
+    </row>
+    <row r="18" spans="1:7" s="162" customFormat="1">
+      <c r="A18" s="159">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B18" s="164" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="165"/>
+      <c r="D18" s="165"/>
+      <c r="E18" s="165"/>
+      <c r="F18" s="166" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="162" customFormat="1">
+      <c r="A19" s="159">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B19" s="158" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="161">
+        <v>2</v>
+      </c>
+      <c r="D19" s="167">
+        <v>2</v>
+      </c>
+      <c r="E19" s="167" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" s="168" t="s">
+        <v>90</v>
+      </c>
+      <c r="G19" s="78"/>
+    </row>
+    <row r="20" spans="1:7" s="162" customFormat="1">
+      <c r="A20" s="159">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B20" s="158" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="161"/>
+      <c r="D20" s="167"/>
+      <c r="E20" s="167" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" s="168" t="s">
+        <v>115</v>
+      </c>
+      <c r="G20" s="78"/>
+    </row>
+    <row r="21" spans="1:7" s="162" customFormat="1" ht="15" thickBot="1">
+      <c r="A21" s="159">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B21" s="80" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="163"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="167" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" s="168"/>
+    </row>
+    <row r="22" spans="1:7" s="162" customFormat="1">
+      <c r="A22" s="159">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B22" s="164" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="165"/>
+      <c r="D22" s="165"/>
+      <c r="E22" s="165"/>
+      <c r="F22" s="166" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="162" customFormat="1">
+      <c r="A23" s="159">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B23" s="158" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="161">
+        <v>3</v>
+      </c>
+      <c r="D23" s="167">
+        <v>3</v>
+      </c>
+      <c r="E23" s="167" t="s">
+        <v>93</v>
+      </c>
+      <c r="F23" s="168" t="s">
+        <v>90</v>
+      </c>
+      <c r="G23" s="78"/>
+    </row>
+    <row r="24" spans="1:7" s="162" customFormat="1" ht="15" thickBot="1">
+      <c r="A24" s="159">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B24" s="158" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="161"/>
+      <c r="D24" s="167"/>
+      <c r="E24" s="167" t="s">
+        <v>115</v>
+      </c>
+      <c r="F24" s="168" t="s">
+        <v>115</v>
+      </c>
+      <c r="G24" s="78"/>
+    </row>
+    <row r="25" spans="1:7" s="162" customFormat="1">
+      <c r="A25" s="159">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B25" s="164" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="165"/>
+      <c r="D25" s="165"/>
+      <c r="E25" s="165"/>
+      <c r="F25" s="166" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="162" customFormat="1">
+      <c r="A26" s="159">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B26" s="158" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="161">
+        <v>4</v>
+      </c>
+      <c r="D26" s="167">
+        <v>4</v>
+      </c>
+      <c r="E26" s="167" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26" s="168" t="s">
+        <v>90</v>
+      </c>
+      <c r="G26" s="78"/>
+    </row>
+    <row r="27" spans="1:7" s="162" customFormat="1">
+      <c r="A27" s="159">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B27" s="158" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="161"/>
+      <c r="D27" s="167"/>
+      <c r="E27" s="167" t="s">
+        <v>93</v>
+      </c>
+      <c r="F27" s="168" t="s">
+        <v>117</v>
+      </c>
+      <c r="G27" s="78"/>
+    </row>
+    <row r="28" spans="1:7" s="162" customFormat="1">
+      <c r="A28" s="159">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B28" s="158" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="161"/>
+      <c r="D28" s="167"/>
+      <c r="E28" s="167" t="s">
+        <v>93</v>
+      </c>
+      <c r="F28" s="168" t="s">
+        <v>118</v>
+      </c>
+      <c r="G28" s="78"/>
+    </row>
+    <row r="29" spans="1:7" s="162" customFormat="1">
+      <c r="A29" s="159">
+        <f t="shared" ref="A29" si="1">A28+1</f>
+        <v>17</v>
+      </c>
+      <c r="B29" s="158" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="161"/>
+      <c r="D29" s="167"/>
+      <c r="E29" s="167" t="s">
+        <v>115</v>
+      </c>
+      <c r="F29" s="168" t="s">
+        <v>115</v>
+      </c>
+      <c r="G29" s="78"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="12"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{78D0221C-50D4-564C-92BB-63EECF94C98C}">
+          <x14:formula1>
+            <xm:f>Config!$B$2:$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>C7</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>

</xml_diff>